<commit_message>
testing survey DB alex
</commit_message>
<xml_diff>
--- a/data/corvina_length_monthly_2012.xlsx
+++ b/data/corvina_length_monthly_2012.xlsx
@@ -1,22 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27217"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexandrasmith/Documents/GP_git/nicoyafisheries.github.io/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="14100"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="24000" windowHeight="14100"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -38,7 +44,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -354,19 +360,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C448"/>
+  <dimension ref="A1:C449"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G445" sqref="G445"/>
+    <sheetView tabSelected="1" topLeftCell="A402" workbookViewId="0">
+      <selection activeCell="C450" sqref="C450"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" customWidth="1"/>
+    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -377,7 +383,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>40909</v>
       </c>
@@ -388,7 +394,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>40909</v>
       </c>
@@ -399,7 +405,7 @@
         <v>9.6153999999999993</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>40909</v>
       </c>
@@ -410,7 +416,7 @@
         <v>17.692</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>40909</v>
       </c>
@@ -421,7 +427,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>40909</v>
       </c>
@@ -432,7 +438,7 @@
         <v>1.5385</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>40909</v>
       </c>
@@ -443,7 +449,7 @@
         <v>2.6922999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>40909</v>
       </c>
@@ -454,7 +460,7 @@
         <v>1.1537999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>40909</v>
       </c>
@@ -465,7 +471,7 @@
         <v>3.4615</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>40909</v>
       </c>
@@ -476,7 +482,7 @@
         <v>4.1566000000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>40909</v>
       </c>
@@ -487,7 +493,7 @@
         <v>4.1566000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>40909</v>
       </c>
@@ -498,7 +504,7 @@
         <v>6.3875000000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>40909</v>
       </c>
@@ -509,7 +515,7 @@
         <v>2.6694</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>40909</v>
       </c>
@@ -520,7 +526,7 @@
         <v>1.1820999999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>40909</v>
       </c>
@@ -531,7 +537,7 @@
         <v>3.0411999999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>40909</v>
       </c>
@@ -542,7 +548,7 @@
         <v>5.6437999999999997</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>40909</v>
       </c>
@@ -553,7 +559,7 @@
         <v>1.9258</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>40909</v>
       </c>
@@ -564,7 +570,7 @@
         <v>11.221</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>40909</v>
       </c>
@@ -575,7 +581,7 @@
         <v>6.7592999999999996</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>40909</v>
       </c>
@@ -586,7 +592,7 @@
         <v>4.5284000000000004</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>40909</v>
       </c>
@@ -597,7 +603,7 @@
         <v>1.9258</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>40909</v>
       </c>
@@ -608,7 +614,7 @@
         <v>1.1820999999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>40909</v>
       </c>
@@ -619,7 +625,7 @@
         <v>3.7848000000000002</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>40909</v>
       </c>
@@ -630,7 +636,7 @@
         <v>4.1566000000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>40909</v>
       </c>
@@ -641,7 +647,7 @@
         <v>1.554</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>40909</v>
       </c>
@@ -652,7 +658,7 @@
         <v>1.9258</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>40909</v>
       </c>
@@ -663,7 +669,7 @@
         <v>4.5284000000000004</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>40909</v>
       </c>
@@ -674,7 +680,7 @@
         <v>5.6437999999999997</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>40909</v>
       </c>
@@ -685,7 +691,7 @@
         <v>1.554</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>40909</v>
       </c>
@@ -696,7 +702,7 @@
         <v>1.1820999999999999</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>40909</v>
       </c>
@@ -707,7 +713,7 @@
         <v>5.6437999999999997</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>40909</v>
       </c>
@@ -718,7 +724,7 @@
         <v>2.6694</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>40909</v>
       </c>
@@ -729,7 +735,7 @@
         <v>4.5284000000000004</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>40909</v>
       </c>
@@ -740,7 +746,7 @@
         <v>3.7848000000000002</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>40909</v>
       </c>
@@ -751,7 +757,7 @@
         <v>2.6694</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>40909</v>
       </c>
@@ -762,7 +768,7 @@
         <v>2.6694</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>40909</v>
       </c>
@@ -773,7 +779,7 @@
         <v>1.1820999999999999</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>40909</v>
       </c>
@@ -784,7 +790,7 @@
         <v>1.9258</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>40909</v>
       </c>
@@ -795,7 +801,7 @@
         <v>4.5284000000000004</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>40909</v>
       </c>
@@ -806,7 +812,7 @@
         <v>4.1566000000000001</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>40909</v>
       </c>
@@ -817,7 +823,7 @@
         <v>4.5284000000000004</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>40909</v>
       </c>
@@ -828,7 +834,7 @@
         <v>2.2976000000000001</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>40909</v>
       </c>
@@ -839,7 +845,7 @@
         <v>2.2976000000000001</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>40909</v>
       </c>
@@ -850,7 +856,7 @@
         <v>3.7848000000000002</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>40909</v>
       </c>
@@ -861,7 +867,7 @@
         <v>2.2976000000000001</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>40909</v>
       </c>
@@ -872,7 +878,7 @@
         <v>2.2976000000000001</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>40909</v>
       </c>
@@ -883,7 +889,7 @@
         <v>1.554</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>40909</v>
       </c>
@@ -894,7 +900,7 @@
         <v>4.1566000000000001</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>40909</v>
       </c>
@@ -905,7 +911,7 @@
         <v>6.7592999999999996</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>40909</v>
       </c>
@@ -916,7 +922,7 @@
         <v>6.0156999999999998</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>40909</v>
       </c>
@@ -927,7 +933,7 @@
         <v>3.0411999999999999</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>40909</v>
       </c>
@@ -938,7 +944,7 @@
         <v>10.106</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>40909</v>
       </c>
@@ -949,7 +955,7 @@
         <v>2.6694</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>40909</v>
       </c>
@@ -960,7 +966,7 @@
         <v>1.554</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>40909</v>
       </c>
@@ -971,7 +977,7 @@
         <v>1.9258</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>40909</v>
       </c>
@@ -982,7 +988,7 @@
         <v>3.7848000000000002</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>40909</v>
       </c>
@@ -993,7 +999,7 @@
         <v>3.7848000000000002</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>40909</v>
       </c>
@@ -1004,7 +1010,7 @@
         <v>1.9258</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>40909</v>
       </c>
@@ -1015,7 +1021,7 @@
         <v>3.4129999999999998</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>40909</v>
       </c>
@@ -1026,7 +1032,7 @@
         <v>3.0411999999999999</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>40909</v>
       </c>
@@ -1037,7 +1043,7 @@
         <v>1.9258</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>40909</v>
       </c>
@@ -1048,7 +1054,7 @@
         <v>1.9258</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>40940</v>
       </c>
@@ -1059,7 +1065,7 @@
         <v>1.6802999999999999</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>40940</v>
       </c>
@@ -1070,7 +1076,7 @@
         <v>2.8342999999999998</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>40940</v>
       </c>
@@ -1081,7 +1087,7 @@
         <v>5.1386000000000003</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>40940</v>
       </c>
@@ -1092,7 +1098,7 @@
         <v>3.9939</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>40940</v>
       </c>
@@ -1103,7 +1109,7 @@
         <v>13.193</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>40940</v>
       </c>
@@ -1114,7 +1120,7 @@
         <v>15.114000000000001</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>40940</v>
       </c>
@@ -1125,7 +1131,7 @@
         <v>25.079000000000001</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>40940</v>
       </c>
@@ -1136,7 +1142,7 @@
         <v>1.7138</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>40940</v>
       </c>
@@ -1147,7 +1153,7 @@
         <v>5.1666999999999996</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>40940</v>
       </c>
@@ -1158,7 +1164,7 @@
         <v>11.301</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>40940</v>
       </c>
@@ -1169,7 +1175,7 @@
         <v>4.0259</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>40940</v>
       </c>
@@ -1180,7 +1186,7 @@
         <v>12.842000000000001</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>40940</v>
       </c>
@@ -1191,7 +1197,7 @@
         <v>12.848000000000001</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>40940</v>
       </c>
@@ -1202,7 +1208,7 @@
         <v>8.2543000000000006</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>40940</v>
       </c>
@@ -1213,7 +1219,7 @@
         <v>10.175000000000001</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>40940</v>
       </c>
@@ -1224,7 +1230,7 @@
         <v>13.627000000000001</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>40940</v>
       </c>
@@ -1235,7 +1241,7 @@
         <v>14.782</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>40940</v>
       </c>
@@ -1246,7 +1252,7 @@
         <v>8.6569000000000003</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>40940</v>
       </c>
@@ -1257,7 +1263,7 @@
         <v>18.239999999999998</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <v>40940</v>
       </c>
@@ -1268,7 +1274,7 @@
         <v>24.757000000000001</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
         <v>40940</v>
       </c>
@@ -1279,7 +1285,7 @@
         <v>14.034000000000001</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
         <v>40940</v>
       </c>
@@ -1290,7 +1296,7 @@
         <v>18.254000000000001</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
         <v>40940</v>
       </c>
@@ -1301,7 +1307,7 @@
         <v>12.895</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
         <v>40940</v>
       </c>
@@ -1312,7 +1318,7 @@
         <v>28.606999999999999</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
         <v>40940</v>
       </c>
@@ -1323,7 +1329,7 @@
         <v>14.054</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
         <v>40940</v>
       </c>
@@ -1334,7 +1340,7 @@
         <v>21.721</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
         <v>40940</v>
       </c>
@@ -1345,7 +1351,7 @@
         <v>9.4652999999999992</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
         <v>40940</v>
       </c>
@@ -1356,7 +1362,7 @@
         <v>20.198</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
         <v>40940</v>
       </c>
@@ -1367,7 +1373,7 @@
         <v>10.624000000000001</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
         <v>40940</v>
       </c>
@@ -1378,7 +1384,7 @@
         <v>16.760000000000002</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
         <v>40940</v>
       </c>
@@ -1389,7 +1395,7 @@
         <v>8.3346999999999998</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
         <v>40940</v>
       </c>
@@ -1400,7 +1406,7 @@
         <v>9.1064000000000007</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" s="1">
         <v>40940</v>
       </c>
@@ -1411,7 +1417,7 @@
         <v>7.1939000000000002</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" s="1">
         <v>40940</v>
       </c>
@@ -1422,7 +1428,7 @@
         <v>7.5824999999999996</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" s="1">
         <v>40940</v>
       </c>
@@ -1433,7 +1439,7 @@
         <v>12.185</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" s="1">
         <v>40940</v>
       </c>
@@ -1444,7 +1450,7 @@
         <v>17.934999999999999</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" s="1">
         <v>40940</v>
       </c>
@@ -1455,7 +1461,7 @@
         <v>0.70099</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" s="1">
         <v>40940</v>
       </c>
@@ -1466,7 +1472,7 @@
         <v>2.2382</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" s="1">
         <v>40940</v>
       </c>
@@ -1477,7 +1483,7 @@
         <v>3.3915000000000002</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102" s="1">
         <v>40940</v>
       </c>
@@ -1488,7 +1494,7 @@
         <v>5.6948999999999996</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103" s="1">
         <v>40940</v>
       </c>
@@ -1499,7 +1505,7 @@
         <v>0.71972000000000003</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A104" s="1">
         <v>40940</v>
       </c>
@@ -1510,7 +1516,7 @@
         <v>1.4899</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A105" s="1">
         <v>40940</v>
       </c>
@@ -1521,7 +1527,7 @@
         <v>3.411</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A106" s="1">
         <v>40940</v>
       </c>
@@ -1532,7 +1538,7 @@
         <v>2.2663000000000002</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A107" s="1">
         <v>40940</v>
       </c>
@@ -1543,7 +1549,7 @@
         <v>5.7183000000000002</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A108" s="1">
         <v>40940</v>
       </c>
@@ -1554,7 +1560,7 @@
         <v>1.5085999999999999</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A109" s="1">
         <v>40940</v>
       </c>
@@ -1565,7 +1571,7 @@
         <v>11.092000000000001</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A110" s="1">
         <v>40940</v>
       </c>
@@ -1576,7 +1582,7 @@
         <v>2.6680999999999999</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A111" s="1">
         <v>40940</v>
       </c>
@@ -1587,7 +1593,7 @@
         <v>1.5226</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A112" s="1">
         <v>40940</v>
       </c>
@@ -1598,7 +1604,7 @@
         <v>8.4236000000000004</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A113" s="1">
         <v>40940</v>
       </c>
@@ -1609,7 +1615,7 @@
         <v>3.8308</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A114" s="1">
         <v>40940</v>
       </c>
@@ -1620,7 +1626,7 @@
         <v>6.9013</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A115" s="1">
         <v>40940</v>
       </c>
@@ -1631,7 +1637,7 @@
         <v>7.6714000000000002</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A116" s="1">
         <v>40940</v>
       </c>
@@ -1642,7 +1648,7 @@
         <v>2.6962000000000002</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A117" s="1">
         <v>40940</v>
       </c>
@@ -1653,7 +1659,7 @@
         <v>6.5321999999999996</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A118" s="1">
         <v>40940</v>
       </c>
@@ -1664,7 +1670,7 @@
         <v>2.3224999999999998</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A119" s="1">
         <v>40940</v>
       </c>
@@ -1675,7 +1681,7 @@
         <v>3.4773000000000001</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A120" s="1">
         <v>40940</v>
       </c>
@@ -1686,7 +1692,7 @@
         <v>5.7792000000000003</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A121" s="1">
         <v>40940</v>
       </c>
@@ -1697,7 +1703,7 @@
         <v>6.9348000000000001</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A122" s="1">
         <v>40940</v>
       </c>
@@ -1708,7 +1714,7 @@
         <v>4.2576000000000001</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A123" s="1">
         <v>40940</v>
       </c>
@@ -1719,7 +1725,7 @@
         <v>3.4952000000000001</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A124" s="1">
         <v>40940</v>
       </c>
@@ -1730,7 +1736,7 @@
         <v>1.5851</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A125" s="1">
         <v>40940</v>
       </c>
@@ -1741,7 +1747,7 @@
         <v>3.1223000000000001</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A126" s="1">
         <v>40940</v>
       </c>
@@ -1752,7 +1758,7 @@
         <v>2.7429999999999999</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A127" s="1">
         <v>40940</v>
       </c>
@@ -1763,7 +1769,7 @@
         <v>2.7477</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A128" s="1">
         <v>40940</v>
       </c>
@@ -1774,7 +1780,7 @@
         <v>1.6037999999999999</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A129" s="1">
         <v>40940</v>
       </c>
@@ -1785,7 +1791,7 @@
         <v>2.7570999999999999</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A130" s="1">
         <v>40940</v>
       </c>
@@ -1796,7 +1802,7 @@
         <v>2.7625000000000002</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A131" s="1">
         <v>40940</v>
       </c>
@@ -1807,7 +1813,7 @@
         <v>1.2394000000000001</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A132" s="1">
         <v>40969</v>
       </c>
@@ -1818,7 +1824,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A133" s="1">
         <v>40969</v>
       </c>
@@ -1829,7 +1835,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A134" s="1">
         <v>40969</v>
       </c>
@@ -1840,7 +1846,7 @@
         <v>5.85</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A135" s="1">
         <v>40969</v>
       </c>
@@ -1851,7 +1857,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A136" s="1">
         <v>40969</v>
       </c>
@@ -1862,7 +1868,7 @@
         <v>2.85</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A137" s="1">
         <v>40969</v>
       </c>
@@ -1873,7 +1879,7 @@
         <v>10.8</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A138" s="1">
         <v>40969</v>
       </c>
@@ -1884,7 +1890,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A139" s="1">
         <v>40969</v>
       </c>
@@ -1895,7 +1901,7 @@
         <v>3.9</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A140" s="1">
         <v>40969</v>
       </c>
@@ -1906,7 +1912,7 @@
         <v>3.9</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A141" s="1">
         <v>40969</v>
       </c>
@@ -1917,7 +1923,7 @@
         <v>1.65</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A142" s="1">
         <v>40969</v>
       </c>
@@ -1928,7 +1934,7 @@
         <v>8.85</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A143" s="1">
         <v>40969</v>
       </c>
@@ -1939,7 +1945,7 @@
         <v>2.7</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A144" s="1">
         <v>40969</v>
       </c>
@@ -1950,7 +1956,7 @@
         <v>6.75</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A145" s="1">
         <v>40969</v>
       </c>
@@ -1961,7 +1967,7 @@
         <v>2.85</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A146" s="1">
         <v>40969</v>
       </c>
@@ -1972,7 +1978,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A147" s="1">
         <v>40969</v>
       </c>
@@ -1983,7 +1989,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A148" s="1">
         <v>40969</v>
       </c>
@@ -1994,7 +2000,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A149" s="1">
         <v>40969</v>
       </c>
@@ -2005,7 +2011,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A150" s="1">
         <v>40969</v>
       </c>
@@ -2016,7 +2022,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A151" s="1">
         <v>40969</v>
       </c>
@@ -2027,7 +2033,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A152" s="1">
         <v>40969</v>
       </c>
@@ -2038,7 +2044,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A153" s="1">
         <v>40969</v>
       </c>
@@ -2049,7 +2055,7 @@
         <v>2.85</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A154" s="1">
         <v>40969</v>
       </c>
@@ -2060,7 +2066,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A155" s="1">
         <v>40969</v>
       </c>
@@ -2071,7 +2077,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A156" s="1">
         <v>40969</v>
       </c>
@@ -2082,7 +2088,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A157" s="1">
         <v>40969</v>
       </c>
@@ -2093,7 +2099,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A158" s="1">
         <v>40969</v>
       </c>
@@ -2104,7 +2110,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A159" s="1">
         <v>40969</v>
       </c>
@@ -2115,7 +2121,7 @@
         <v>1.95</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A160" s="1">
         <v>40969</v>
       </c>
@@ -2126,7 +2132,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A161" s="1">
         <v>40969</v>
       </c>
@@ -2137,7 +2143,7 @@
         <v>1.95</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A162" s="1">
         <v>40969</v>
       </c>
@@ -2148,7 +2154,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A163" s="1">
         <v>40969</v>
       </c>
@@ -2159,7 +2165,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A164" s="1">
         <v>40969</v>
       </c>
@@ -2170,7 +2176,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A165" s="1">
         <v>40969</v>
       </c>
@@ -2181,7 +2187,7 @@
         <v>1.65</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A166" s="1">
         <v>40969</v>
       </c>
@@ -2192,7 +2198,7 @@
         <v>2.85</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A167" s="1">
         <v>40969</v>
       </c>
@@ -2203,7 +2209,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A168" s="1">
         <v>40969</v>
       </c>
@@ -2214,7 +2220,7 @@
         <v>2.85</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A169" s="1">
         <v>40969</v>
       </c>
@@ -2225,7 +2231,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A170" s="1">
         <v>40969</v>
       </c>
@@ -2236,7 +2242,7 @@
         <v>5.0999999999999996</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A171" s="1">
         <v>40969</v>
       </c>
@@ -2247,7 +2253,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A172" s="1">
         <v>40969</v>
       </c>
@@ -2258,7 +2264,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A173" s="1">
         <v>40969</v>
       </c>
@@ -2269,7 +2275,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A174" s="1">
         <v>40969</v>
       </c>
@@ -2280,7 +2286,7 @@
         <v>4.05</v>
       </c>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A175" s="1">
         <v>40969</v>
       </c>
@@ -2291,7 +2297,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A176" s="1">
         <v>40969</v>
       </c>
@@ -2302,7 +2308,7 @@
         <v>1.65</v>
       </c>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A177" s="1">
         <v>40969</v>
       </c>
@@ -2313,7 +2319,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A178" s="1">
         <v>40969</v>
       </c>
@@ -2324,7 +2330,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A179" s="1">
         <v>40969</v>
       </c>
@@ -2335,7 +2341,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A180" s="1">
         <v>40969</v>
       </c>
@@ -2346,7 +2352,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A181" s="1">
         <v>40969</v>
       </c>
@@ -2357,7 +2363,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A182" s="1">
         <v>40969</v>
       </c>
@@ -2368,7 +2374,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A183" s="1">
         <v>40969</v>
       </c>
@@ -2379,7 +2385,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A184" s="1">
         <v>40969</v>
       </c>
@@ -2390,7 +2396,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A185" s="1">
         <v>41000</v>
       </c>
@@ -2401,7 +2407,7 @@
         <v>1.3092999999999999</v>
       </c>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A186" s="1">
         <v>41000</v>
       </c>
@@ -2412,7 +2418,7 @@
         <v>2.2374999999999998</v>
       </c>
     </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A187" s="1">
         <v>41000</v>
       </c>
@@ -2423,7 +2429,7 @@
         <v>1.4994000000000001</v>
       </c>
     </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A188" s="1">
         <v>41000</v>
       </c>
@@ -2434,7 +2440,7 @@
         <v>2.2422</v>
       </c>
     </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A189" s="1">
         <v>41000</v>
       </c>
@@ -2445,7 +2451,7 @@
         <v>4.8399000000000001</v>
       </c>
     </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A190" s="1">
         <v>41000</v>
       </c>
@@ -2456,7 +2462,7 @@
         <v>3.1749999999999998</v>
       </c>
     </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A191" s="1">
         <v>41000</v>
       </c>
@@ -2467,7 +2473,7 @@
         <v>3.1776</v>
       </c>
     </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A192" s="1">
         <v>41000</v>
       </c>
@@ -2478,7 +2484,7 @@
         <v>3.3651</v>
       </c>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A193" s="1">
         <v>41000</v>
       </c>
@@ -2489,7 +2495,7 @@
         <v>5.4044999999999996</v>
       </c>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A194" s="1">
         <v>41000</v>
       </c>
@@ -2500,7 +2506,7 @@
         <v>1.3327</v>
       </c>
     </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A195" s="1">
         <v>41000</v>
       </c>
@@ -2511,7 +2517,7 @@
         <v>3.3719999999999999</v>
       </c>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A196" s="1">
         <v>41000</v>
       </c>
@@ -2522,7 +2528,7 @@
         <v>8.1891999999999996</v>
       </c>
     </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A197" s="1">
         <v>41000</v>
       </c>
@@ -2533,7 +2539,7 @@
         <v>4.1177000000000001</v>
       </c>
     </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A198" s="1">
         <v>41000</v>
       </c>
@@ -2544,7 +2550,7 @@
         <v>3.1938</v>
       </c>
     </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A199" s="1">
         <v>41000</v>
       </c>
@@ -2555,7 +2561,7 @@
         <v>3.9367999999999999</v>
       </c>
     </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A200" s="1">
         <v>41000</v>
       </c>
@@ -2566,7 +2572,7 @@
         <v>3.9394</v>
       </c>
     </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A201" s="1">
         <v>41000</v>
       </c>
@@ -2577,7 +2583,7 @@
         <v>7.2754000000000003</v>
       </c>
     </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A202" s="1">
         <v>41000</v>
       </c>
@@ -2588,7 +2594,7 @@
         <v>3.2029999999999998</v>
       </c>
     </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A203" s="1">
         <v>41000</v>
       </c>
@@ -2599,7 +2605,7 @@
         <v>14.317</v>
       </c>
     </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A204" s="1">
         <v>41000</v>
       </c>
@@ -2610,7 +2616,7 @@
         <v>6.3560999999999996</v>
       </c>
     </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A205" s="1">
         <v>41000</v>
       </c>
@@ -2621,7 +2627,7 @@
         <v>8.0248000000000008</v>
       </c>
     </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A206" s="1">
         <v>41000</v>
       </c>
@@ -2632,7 +2638,7 @@
         <v>13.212999999999999</v>
       </c>
     </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A207" s="1">
         <v>41000</v>
       </c>
@@ -2643,7 +2649,7 @@
         <v>3.0297000000000001</v>
       </c>
     </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A208" s="1">
         <v>41000</v>
       </c>
@@ -2654,7 +2660,7 @@
         <v>12.292</v>
       </c>
     </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A209" s="1">
         <v>41000</v>
       </c>
@@ -2665,7 +2671,7 @@
         <v>16.922999999999998</v>
       </c>
     </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A210" s="1">
         <v>41000</v>
       </c>
@@ -2676,7 +2682,7 @@
         <v>8.0368999999999993</v>
       </c>
     </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A211" s="1">
         <v>41000</v>
       </c>
@@ -2687,7 +2693,7 @@
         <v>8.0391999999999992</v>
       </c>
     </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A212" s="1">
         <v>41000</v>
       </c>
@@ -2698,7 +2704,7 @@
         <v>11.19</v>
       </c>
     </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A213" s="1">
         <v>41000</v>
       </c>
@@ -2709,7 +2715,7 @@
         <v>16.748000000000001</v>
       </c>
     </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A214" s="1">
         <v>41000</v>
       </c>
@@ -2720,7 +2726,7 @@
         <v>13.787000000000001</v>
       </c>
     </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A215" s="1">
         <v>41000</v>
       </c>
@@ -2731,7 +2737,7 @@
         <v>3.9744000000000002</v>
       </c>
     </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A216" s="1">
         <v>41000</v>
       </c>
@@ -2742,7 +2748,7 @@
         <v>14.347</v>
       </c>
     </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A217" s="1">
         <v>41000</v>
       </c>
@@ -2753,7 +2759,7 @@
         <v>8.0531000000000006</v>
       </c>
     </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A218" s="1">
         <v>41000</v>
       </c>
@@ -2764,7 +2770,7 @@
         <v>6.3890000000000002</v>
       </c>
     </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A219" s="1">
         <v>41000</v>
       </c>
@@ -2775,7 +2781,7 @@
         <v>12.132</v>
       </c>
     </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A220" s="1">
         <v>41000</v>
       </c>
@@ -2786,7 +2792,7 @@
         <v>6.0232999999999999</v>
       </c>
     </row>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A221" s="1">
         <v>41000</v>
       </c>
@@ -2797,7 +2803,7 @@
         <v>8.0625999999999998</v>
       </c>
     </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A222" s="1">
         <v>41000</v>
       </c>
@@ -2808,7 +2814,7 @@
         <v>7.1387</v>
       </c>
     </row>
-    <row r="223" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A223" s="1">
         <v>41000</v>
       </c>
@@ -2819,7 +2825,7 @@
         <v>5.1043000000000003</v>
       </c>
     </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A224" s="1">
         <v>41000</v>
       </c>
@@ -2830,7 +2836,7 @@
         <v>7.1436000000000002</v>
       </c>
     </row>
-    <row r="225" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A225" s="1">
         <v>41000</v>
       </c>
@@ -2841,7 +2847,7 @@
         <v>6.4055</v>
       </c>
     </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A226" s="1">
         <v>41000</v>
       </c>
@@ -2852,7 +2858,7 @@
         <v>8.0741999999999994</v>
       </c>
     </row>
-    <row r="227" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A227" s="1">
         <v>41000</v>
       </c>
@@ -2863,7 +2869,7 @@
         <v>7.3360000000000003</v>
       </c>
     </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A228" s="1">
         <v>41000</v>
       </c>
@@ -2874,7 +2880,7 @@
         <v>4.0049999999999999</v>
       </c>
     </row>
-    <row r="229" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A229" s="1">
         <v>41000</v>
       </c>
@@ -2885,7 +2891,7 @@
         <v>4.1924999999999999</v>
       </c>
     </row>
-    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A230" s="1">
         <v>41000</v>
       </c>
@@ -2896,7 +2902,7 @@
         <v>8.8245000000000005</v>
       </c>
     </row>
-    <row r="231" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A231" s="1">
         <v>41000</v>
       </c>
@@ -2907,7 +2913,7 @@
         <v>8.8268000000000004</v>
       </c>
     </row>
-    <row r="232" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A232" s="1">
         <v>41000</v>
       </c>
@@ -2918,7 +2924,7 @@
         <v>2.3479000000000001</v>
       </c>
     </row>
-    <row r="233" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A233" s="1">
         <v>41000</v>
       </c>
@@ -2929,7 +2935,7 @@
         <v>3.2755999999999998</v>
       </c>
     </row>
-    <row r="234" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A234" s="1">
         <v>41000</v>
       </c>
@@ -2940,7 +2946,7 @@
         <v>2.1673</v>
       </c>
     </row>
-    <row r="235" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A235" s="1">
         <v>41000</v>
       </c>
@@ -2951,7 +2957,7 @@
         <v>10.318</v>
       </c>
     </row>
-    <row r="236" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A236" s="1">
         <v>41000</v>
       </c>
@@ -2962,7 +2968,7 @@
         <v>6.4311999999999996</v>
       </c>
     </row>
-    <row r="237" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A237" s="1">
         <v>41000</v>
       </c>
@@ -2973,7 +2979,7 @@
         <v>4.2115999999999998</v>
       </c>
     </row>
-    <row r="238" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A238" s="1">
         <v>41000</v>
       </c>
@@ -2984,7 +2990,7 @@
         <v>7.3643999999999998</v>
       </c>
     </row>
-    <row r="239" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A239" s="1">
         <v>41000</v>
       </c>
@@ -2995,7 +3001,7 @@
         <v>5.3247</v>
       </c>
     </row>
-    <row r="240" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A240" s="1">
         <v>41000</v>
       </c>
@@ -3006,7 +3012,7 @@
         <v>2.3666999999999998</v>
       </c>
     </row>
-    <row r="241" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A241" s="1">
         <v>41000</v>
       </c>
@@ -3017,7 +3023,7 @@
         <v>8.2949000000000002</v>
       </c>
     </row>
-    <row r="242" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A242" s="1">
         <v>41000</v>
       </c>
@@ -3028,7 +3034,7 @@
         <v>2.1861000000000002</v>
       </c>
     </row>
-    <row r="243" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A243" s="1">
         <v>41000</v>
       </c>
@@ -3039,7 +3045,7 @@
         <v>1.6326000000000001</v>
       </c>
     </row>
-    <row r="244" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A244" s="1">
         <v>41000</v>
       </c>
@@ -3050,7 +3056,7 @@
         <v>2.3759000000000001</v>
       </c>
     </row>
-    <row r="245" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A245" s="1">
         <v>41000</v>
       </c>
@@ -3061,7 +3067,7 @@
         <v>1.4522999999999999</v>
       </c>
     </row>
-    <row r="246" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A246" s="1">
         <v>41000</v>
       </c>
@@ -3072,7 +3078,7 @@
         <v>4.0472000000000001</v>
       </c>
     </row>
-    <row r="247" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A247" s="1">
         <v>41000</v>
       </c>
@@ -3083,7 +3089,7 @@
         <v>2.3828999999999998</v>
       </c>
     </row>
-    <row r="248" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A248" s="1">
         <v>41000</v>
       </c>
@@ -3094,7 +3100,7 @@
         <v>1.4661999999999999</v>
       </c>
     </row>
-    <row r="249" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A249" s="1">
         <v>41030</v>
       </c>
@@ -3105,7 +3111,7 @@
         <v>0.99328000000000005</v>
       </c>
     </row>
-    <row r="250" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A250" s="1">
         <v>41030</v>
       </c>
@@ -3116,7 +3122,7 @@
         <v>2.1402000000000001</v>
       </c>
     </row>
-    <row r="251" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A251" s="1">
         <v>41030</v>
       </c>
@@ -3127,7 +3133,7 @@
         <v>2.1364000000000001</v>
       </c>
     </row>
-    <row r="252" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A252" s="1">
         <v>41030</v>
       </c>
@@ -3138,7 +3144,7 @@
         <v>2.9979</v>
       </c>
     </row>
-    <row r="253" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A253" s="1">
         <v>41030</v>
       </c>
@@ -3149,7 +3155,7 @@
         <v>0.97521999999999998</v>
       </c>
     </row>
-    <row r="254" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A254" s="1">
         <v>41030</v>
       </c>
@@ -3160,7 +3166,7 @@
         <v>2.9906000000000001</v>
       </c>
     </row>
-    <row r="255" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A255" s="1">
         <v>41030</v>
       </c>
@@ -3171,7 +3177,7 @@
         <v>1.1116999999999999</v>
       </c>
     </row>
-    <row r="256" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A256" s="1">
         <v>41030</v>
       </c>
@@ -3182,7 +3188,7 @@
         <v>2.1145</v>
       </c>
     </row>
-    <row r="257" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A257" s="1">
         <v>41030</v>
       </c>
@@ -3193,7 +3199,7 @@
         <v>2.1067</v>
       </c>
     </row>
-    <row r="258" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A258" s="1">
         <v>41030</v>
       </c>
@@ -3204,7 +3210,7 @@
         <v>3.9710000000000001</v>
       </c>
     </row>
-    <row r="259" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A259" s="1">
         <v>41030</v>
       </c>
@@ -3215,7 +3221,7 @@
         <v>3.1021000000000001</v>
       </c>
     </row>
-    <row r="260" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A260" s="1">
         <v>41030</v>
       </c>
@@ -3226,7 +3232,7 @@
         <v>7.1367000000000003</v>
       </c>
     </row>
-    <row r="261" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A261" s="1">
         <v>41030</v>
       </c>
@@ -3237,7 +3243,7 @@
         <v>4.2487000000000004</v>
       </c>
     </row>
-    <row r="262" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A262" s="1">
         <v>41030</v>
       </c>
@@ -3248,7 +3254,7 @@
         <v>2.2221000000000002</v>
       </c>
     </row>
-    <row r="263" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A263" s="1">
         <v>41030</v>
       </c>
@@ -3259,7 +3265,7 @@
         <v>3.9495</v>
       </c>
     </row>
-    <row r="264" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A264" s="1">
         <v>41030</v>
       </c>
@@ -3270,7 +3276,7 @@
         <v>2.0710000000000002</v>
       </c>
     </row>
-    <row r="265" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A265" s="1">
         <v>41030</v>
       </c>
@@ -3281,7 +3287,7 @@
         <v>3.0768</v>
       </c>
     </row>
-    <row r="266" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A266" s="1">
         <v>41030</v>
       </c>
@@ -3292,7 +3298,7 @@
         <v>1.0537000000000001</v>
       </c>
     </row>
-    <row r="267" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A267" s="1">
         <v>41030</v>
       </c>
@@ -3303,7 +3309,7 @@
         <v>3.9344000000000001</v>
       </c>
     </row>
-    <row r="268" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A268" s="1">
         <v>41030</v>
       </c>
@@ -3314,7 +3320,7 @@
         <v>12.872999999999999</v>
       </c>
     </row>
-    <row r="269" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A269" s="1">
         <v>41030</v>
       </c>
@@ -3325,7 +3331,7 @@
         <v>3.0617000000000001</v>
       </c>
     </row>
-    <row r="270" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A270" s="1">
         <v>41030</v>
       </c>
@@ -3336,7 +3342,7 @@
         <v>7.9621000000000004</v>
       </c>
     </row>
-    <row r="271" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A271" s="1">
         <v>41030</v>
       </c>
@@ -3347,7 +3353,7 @@
         <v>0.89053000000000004</v>
       </c>
     </row>
-    <row r="272" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A272" s="1">
         <v>41030</v>
       </c>
@@ -3358,7 +3364,7 @@
         <v>5.9352</v>
       </c>
     </row>
-    <row r="273" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A273" s="1">
         <v>41030</v>
       </c>
@@ -3369,7 +3375,7 @@
         <v>6.0759999999999996</v>
       </c>
     </row>
-    <row r="274" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A274" s="1">
         <v>41030</v>
       </c>
@@ -3380,7 +3386,7 @@
         <v>0.87978999999999996</v>
       </c>
     </row>
-    <row r="275" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A275" s="1">
         <v>41030</v>
       </c>
@@ -3391,7 +3397,7 @@
         <v>5.9244000000000003</v>
       </c>
     </row>
-    <row r="276" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A276" s="1">
         <v>41030</v>
       </c>
@@ -3402,7 +3408,7 @@
         <v>3.0364</v>
       </c>
     </row>
-    <row r="277" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A277" s="1">
         <v>41030</v>
       </c>
@@ -3413,7 +3419,7 @@
         <v>6.7828999999999997</v>
       </c>
     </row>
-    <row r="278" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A278" s="1">
         <v>41030</v>
       </c>
@@ -3424,7 +3430,7 @@
         <v>3.0291000000000001</v>
       </c>
     </row>
-    <row r="279" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A279" s="1">
         <v>41030</v>
       </c>
@@ -3435,7 +3441,7 @@
         <v>3.8906000000000001</v>
       </c>
     </row>
-    <row r="280" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A280" s="1">
         <v>41030</v>
       </c>
@@ -3446,7 +3452,7 @@
         <v>2.1564000000000001</v>
       </c>
     </row>
-    <row r="281" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A281" s="1">
         <v>41030</v>
       </c>
@@ -3457,7 +3463,7 @@
         <v>2.1528999999999998</v>
       </c>
     </row>
-    <row r="282" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A282" s="1">
         <v>41030</v>
       </c>
@@ -3468,7 +3474,7 @@
         <v>3.8797999999999999</v>
       </c>
     </row>
-    <row r="283" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A283" s="1">
         <v>41030</v>
       </c>
@@ -3479,7 +3485,7 @@
         <v>0.84711000000000003</v>
       </c>
     </row>
-    <row r="284" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A284" s="1">
         <v>41030</v>
       </c>
@@ -3490,7 +3496,7 @@
         <v>3.1514000000000002</v>
       </c>
     </row>
-    <row r="285" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A285" s="1">
         <v>41030</v>
       </c>
@@ -3501,7 +3507,7 @@
         <v>4.7348999999999997</v>
       </c>
     </row>
-    <row r="286" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A286" s="1">
         <v>41030</v>
       </c>
@@ -3512,7 +3518,7 @@
         <v>2.9998</v>
       </c>
     </row>
-    <row r="287" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A287" s="1">
         <v>41030</v>
       </c>
@@ -3523,7 +3529,7 @@
         <v>5.8810000000000002</v>
       </c>
     </row>
-    <row r="288" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A288" s="1">
         <v>41030</v>
       </c>
@@ -3534,7 +3540,7 @@
         <v>2.9921000000000002</v>
       </c>
     </row>
-    <row r="289" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A289" s="1">
         <v>41030</v>
       </c>
@@ -3545,7 +3551,7 @@
         <v>3.1328999999999998</v>
       </c>
     </row>
-    <row r="290" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A290" s="1">
         <v>41030</v>
       </c>
@@ -3556,7 +3562,7 @@
         <v>0.82132000000000005</v>
       </c>
     </row>
-    <row r="291" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A291" s="1">
         <v>41030</v>
       </c>
@@ -3567,7 +3573,7 @@
         <v>2.1120999999999999</v>
       </c>
     </row>
-    <row r="292" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A292" s="1">
         <v>41030</v>
       </c>
@@ -3578,7 +3584,7 @@
         <v>2.1091000000000002</v>
       </c>
     </row>
-    <row r="293" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A293" s="1">
         <v>41030</v>
       </c>
@@ -3589,7 +3595,7 @@
         <v>1.9604999999999999</v>
       </c>
     </row>
-    <row r="294" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A294" s="1">
         <v>41030</v>
       </c>
@@ -3600,7 +3606,7 @@
         <v>2.9662999999999999</v>
       </c>
     </row>
-    <row r="295" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A295" s="1">
         <v>41030</v>
       </c>
@@ -3611,7 +3617,7 @@
         <v>1.9498</v>
       </c>
     </row>
-    <row r="296" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A296" s="1">
         <v>41030</v>
       </c>
@@ -3622,7 +3628,7 @@
         <v>1.9352</v>
       </c>
     </row>
-    <row r="297" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A297" s="1">
         <v>41030</v>
       </c>
@@ -3633,7 +3639,7 @@
         <v>2.9379</v>
       </c>
     </row>
-    <row r="298" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A298" s="1">
         <v>41030</v>
       </c>
@@ -3644,7 +3650,7 @@
         <v>0.77059</v>
       </c>
     </row>
-    <row r="299" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A299" s="1">
         <v>41030</v>
       </c>
@@ -3655,7 +3661,7 @@
         <v>1.0444</v>
       </c>
     </row>
-    <row r="300" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A300" s="1">
         <v>41030</v>
       </c>
@@ -3666,7 +3672,7 @@
         <v>0.88129000000000002</v>
       </c>
     </row>
-    <row r="301" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A301" s="1">
         <v>41122</v>
       </c>
@@ -3677,7 +3683,7 @@
         <v>2.3045</v>
       </c>
     </row>
-    <row r="302" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A302" s="1">
         <v>41122</v>
       </c>
@@ -3688,7 +3694,7 @@
         <v>9.1693999999999996</v>
       </c>
     </row>
-    <row r="303" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A303" s="1">
         <v>41122</v>
       </c>
@@ -3699,7 +3705,7 @@
         <v>5.7492999999999999</v>
       </c>
     </row>
-    <row r="304" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A304" s="1">
         <v>41122</v>
       </c>
@@ -3710,7 +3716,7 @@
         <v>16.042000000000002</v>
       </c>
     </row>
-    <row r="305" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A305" s="1">
         <v>41122</v>
       </c>
@@ -3721,7 +3727,7 @@
         <v>21.763000000000002</v>
       </c>
     </row>
-    <row r="306" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A306" s="1">
         <v>41122</v>
       </c>
@@ -3732,7 +3738,7 @@
         <v>27.484000000000002</v>
       </c>
     </row>
-    <row r="307" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A307" s="1">
         <v>41122</v>
       </c>
@@ -3743,7 +3749,7 @@
         <v>30.920999999999999</v>
       </c>
     </row>
-    <row r="308" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A308" s="1">
         <v>41122</v>
       </c>
@@ -3754,7 +3760,7 @@
         <v>43.5</v>
       </c>
     </row>
-    <row r="309" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A309" s="1">
         <v>41122</v>
       </c>
@@ -3765,7 +3771,7 @@
         <v>48.65</v>
       </c>
     </row>
-    <row r="310" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A310" s="1">
         <v>41122</v>
       </c>
@@ -3776,7 +3782,7 @@
         <v>55.515000000000001</v>
       </c>
     </row>
-    <row r="311" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A311" s="1">
         <v>41122</v>
       </c>
@@ -3787,7 +3793,7 @@
         <v>32.093000000000004</v>
       </c>
     </row>
-    <row r="312" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A312" s="1">
         <v>41122</v>
       </c>
@@ -3798,7 +3804,7 @@
         <v>45.814</v>
       </c>
     </row>
-    <row r="313" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A313" s="1">
         <v>41122</v>
       </c>
@@ -3809,7 +3815,7 @@
         <v>31.535</v>
       </c>
     </row>
-    <row r="314" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A314" s="1">
         <v>41122</v>
       </c>
@@ -3820,7 +3826,7 @@
         <v>45.258000000000003</v>
       </c>
     </row>
-    <row r="315" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A315" s="1">
         <v>41122</v>
       </c>
@@ -3831,7 +3837,7 @@
         <v>21.835999999999999</v>
       </c>
     </row>
-    <row r="316" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A316" s="1">
         <v>41122</v>
       </c>
@@ -3842,7 +3848,7 @@
         <v>21.841999999999999</v>
       </c>
     </row>
-    <row r="317" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A317" s="1">
         <v>41122</v>
       </c>
@@ -3853,7 +3859,7 @@
         <v>18.420999999999999</v>
       </c>
     </row>
-    <row r="318" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A318" s="1">
         <v>41122</v>
       </c>
@@ -3864,7 +3870,7 @@
         <v>12.714</v>
       </c>
     </row>
-    <row r="319" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A319" s="1">
         <v>41122</v>
       </c>
@@ -3875,7 +3881,7 @@
         <v>4.1498999999999997</v>
       </c>
     </row>
-    <row r="320" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A320" s="1">
         <v>41122</v>
       </c>
@@ -3886,7 +3892,7 @@
         <v>10.443</v>
       </c>
     </row>
-    <row r="321" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A321" s="1">
         <v>41122</v>
       </c>
@@ -3897,7 +3903,7 @@
         <v>2.4653999999999998</v>
       </c>
     </row>
-    <row r="322" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A322" s="1">
         <v>41122</v>
       </c>
@@ -3908,7 +3914,7 @@
         <v>3.0436999999999999</v>
       </c>
     </row>
-    <row r="323" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A323" s="1">
         <v>41122</v>
       </c>
@@ -3919,7 +3925,7 @@
         <v>4.1942000000000004</v>
       </c>
     </row>
-    <row r="324" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A324" s="1">
         <v>41122</v>
       </c>
@@ -3930,7 +3936,7 @@
         <v>3.0657999999999999</v>
       </c>
     </row>
-    <row r="325" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A325" s="1">
         <v>41122</v>
       </c>
@@ -3941,7 +3947,7 @@
         <v>49.390999999999998</v>
       </c>
     </row>
-    <row r="326" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A326" s="1">
         <v>41122</v>
       </c>
@@ -3952,7 +3958,7 @@
         <v>3.1160999999999999</v>
       </c>
     </row>
-    <row r="327" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A327" s="1">
         <v>41122</v>
       </c>
@@ -3963,7 +3969,7 @@
         <v>3.1236999999999999</v>
       </c>
     </row>
-    <row r="328" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A328" s="1">
         <v>41122</v>
       </c>
@@ -3974,7 +3980,7 @@
         <v>5.4230999999999998</v>
       </c>
     </row>
-    <row r="329" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A329" s="1">
         <v>41122</v>
       </c>
@@ -3985,7 +3991,7 @@
         <v>4.2946999999999997</v>
       </c>
     </row>
-    <row r="330" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A330" s="1">
         <v>41122</v>
       </c>
@@ -3996,7 +4002,7 @@
         <v>3.7378</v>
       </c>
     </row>
-    <row r="331" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A331" s="1">
         <v>41122</v>
       </c>
@@ -4007,7 +4013,7 @@
         <v>4.8959999999999999</v>
       </c>
     </row>
-    <row r="332" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A332" s="1">
         <v>41122</v>
       </c>
@@ -4018,7 +4024,7 @@
         <v>3.7599</v>
       </c>
     </row>
-    <row r="333" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A333" s="1">
         <v>41122</v>
       </c>
@@ -4029,7 +4035,7 @@
         <v>4.9104000000000001</v>
       </c>
     </row>
-    <row r="334" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A334" s="1">
         <v>41122</v>
       </c>
@@ -4040,7 +4046,7 @@
         <v>3.2029000000000001</v>
       </c>
     </row>
-    <row r="335" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A335" s="1">
         <v>41122</v>
       </c>
@@ -4051,7 +4057,7 @@
         <v>3.2105999999999999</v>
       </c>
     </row>
-    <row r="336" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A336" s="1">
         <v>41122</v>
       </c>
@@ -4062,7 +4068,7 @@
         <v>3.2250999999999999</v>
       </c>
     </row>
-    <row r="337" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A337" s="1">
         <v>41122</v>
       </c>
@@ -4073,7 +4079,7 @@
         <v>3.2395999999999998</v>
       </c>
     </row>
-    <row r="338" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A338" s="1">
         <v>41122</v>
       </c>
@@ -4084,7 +4090,7 @@
         <v>5.5610999999999997</v>
       </c>
     </row>
-    <row r="339" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A339" s="1">
         <v>41122</v>
       </c>
@@ -4095,7 +4101,7 @@
         <v>4.9965000000000002</v>
       </c>
     </row>
-    <row r="340" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A340" s="1">
         <v>41122</v>
       </c>
@@ -4106,7 +4112,7 @@
         <v>2.7174999999999998</v>
       </c>
     </row>
-    <row r="341" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A341" s="1">
         <v>41122</v>
       </c>
@@ -4117,7 +4123,7 @@
         <v>6.1538000000000004</v>
       </c>
     </row>
-    <row r="342" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A342" s="1">
         <v>41122</v>
       </c>
@@ -4128,7 +4134,7 @@
         <v>5.59</v>
       </c>
     </row>
-    <row r="343" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A343" s="1">
         <v>41122</v>
       </c>
@@ -4139,7 +4145,7 @@
         <v>3.3111000000000002</v>
       </c>
     </row>
-    <row r="344" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A344" s="1">
         <v>41122</v>
       </c>
@@ -4150,7 +4156,7 @@
         <v>4.4607999999999999</v>
       </c>
     </row>
-    <row r="345" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A345" s="1">
         <v>41122</v>
       </c>
@@ -4161,7 +4167,7 @@
         <v>4.4752999999999998</v>
       </c>
     </row>
-    <row r="346" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A346" s="1">
         <v>41122</v>
       </c>
@@ -4172,7 +4178,7 @@
         <v>3.9260000000000002</v>
       </c>
     </row>
-    <row r="347" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A347" s="1">
         <v>41183</v>
       </c>
@@ -4183,7 +4189,7 @@
         <v>0.87856999999999996</v>
       </c>
     </row>
-    <row r="348" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A348" s="1">
         <v>41183</v>
       </c>
@@ -4194,7 +4200,7 @@
         <v>2.9963000000000002</v>
       </c>
     </row>
-    <row r="349" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A349" s="1">
         <v>41183</v>
       </c>
@@ -4205,7 +4211,7 @@
         <v>3.0950000000000002</v>
       </c>
     </row>
-    <row r="350" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A350" s="1">
         <v>41183</v>
       </c>
@@ -4216,7 +4222,7 @@
         <v>3.1938</v>
       </c>
     </row>
-    <row r="351" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A351" s="1">
         <v>41183</v>
       </c>
@@ -4227,7 +4233,7 @@
         <v>3.0998999999999999</v>
       </c>
     </row>
-    <row r="352" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A352" s="1">
         <v>41183</v>
       </c>
@@ -4238,7 +4244,7 @@
         <v>4.1604999999999999</v>
       </c>
     </row>
-    <row r="353" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A353" s="1">
         <v>41183</v>
       </c>
@@ -4249,7 +4255,7 @@
         <v>0.98933000000000004</v>
       </c>
     </row>
-    <row r="354" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A354" s="1">
         <v>41183</v>
       </c>
@@ -4260,7 +4266,7 @@
         <v>5.1265999999999998</v>
       </c>
     </row>
-    <row r="355" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A355" s="1">
         <v>41183</v>
       </c>
@@ -4271,7 +4277,7 @@
         <v>7.2446999999999999</v>
       </c>
     </row>
-    <row r="356" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A356" s="1">
         <v>41183</v>
       </c>
@@ -4282,7 +4288,7 @@
         <v>0.99677000000000004</v>
       </c>
     </row>
-    <row r="357" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A357" s="1">
         <v>41183</v>
       </c>
@@ -4293,7 +4299,7 @@
         <v>2.0573999999999999</v>
       </c>
     </row>
-    <row r="358" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A358" s="1">
         <v>41183</v>
       </c>
@@ -4304,7 +4310,7 @@
         <v>2.0619000000000001</v>
       </c>
     </row>
-    <row r="359" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A359" s="1">
         <v>41183</v>
       </c>
@@ -4315,7 +4321,7 @@
         <v>4.1797000000000004</v>
       </c>
     </row>
-    <row r="360" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A360" s="1">
         <v>41183</v>
       </c>
@@ -4326,7 +4332,7 @@
         <v>5.1435000000000004</v>
       </c>
     </row>
-    <row r="361" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A361" s="1">
         <v>41183</v>
       </c>
@@ -4337,7 +4343,7 @@
         <v>2.0691000000000002</v>
       </c>
     </row>
-    <row r="362" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A362" s="1">
         <v>41183</v>
       </c>
@@ -4348,7 +4354,7 @@
         <v>3.1291000000000002</v>
       </c>
     </row>
-    <row r="363" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A363" s="1">
         <v>41183</v>
       </c>
@@ -4359,7 +4365,7 @@
         <v>6.3045999999999998</v>
       </c>
     </row>
-    <row r="364" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A364" s="1">
         <v>41183</v>
       </c>
@@ -4370,7 +4376,7 @@
         <v>8.1343999999999994</v>
       </c>
     </row>
-    <row r="365" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A365" s="1">
         <v>41183</v>
       </c>
@@ -4381,7 +4387,7 @@
         <v>3.0404</v>
       </c>
     </row>
-    <row r="366" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A366" s="1">
         <v>41183</v>
       </c>
@@ -4392,7 +4398,7 @@
         <v>7.1776999999999997</v>
       </c>
     </row>
-    <row r="367" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A367" s="1">
         <v>41183</v>
       </c>
@@ -4403,7 +4409,7 @@
         <v>3.1414</v>
       </c>
     </row>
-    <row r="368" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A368" s="1">
         <v>41183</v>
       </c>
@@ -4414,7 +4420,7 @@
         <v>2.0888</v>
       </c>
     </row>
-    <row r="369" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A369" s="1">
         <v>41183</v>
       </c>
@@ -4425,7 +4431,7 @@
         <v>2.1873</v>
       </c>
     </row>
-    <row r="370" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A370" s="1">
         <v>41183</v>
       </c>
@@ -4436,7 +4442,7 @@
         <v>3.1514000000000002</v>
       </c>
     </row>
-    <row r="371" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A371" s="1">
         <v>41183</v>
       </c>
@@ -4447,7 +4453,7 @@
         <v>4.1153000000000004</v>
       </c>
     </row>
-    <row r="372" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A372" s="1">
         <v>41183</v>
       </c>
@@ -4458,7 +4464,7 @@
         <v>1.1364000000000001</v>
       </c>
     </row>
-    <row r="373" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A373" s="1">
         <v>41183</v>
       </c>
@@ -4469,7 +4475,7 @@
         <v>1.2354000000000001</v>
       </c>
     </row>
-    <row r="374" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A374" s="1">
         <v>41183</v>
       </c>
@@ -4480,7 +4486,7 @@
         <v>5.0885999999999996</v>
       </c>
     </row>
-    <row r="375" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A375" s="1">
         <v>41183</v>
       </c>
@@ -4491,7 +4497,7 @@
         <v>2.11</v>
       </c>
     </row>
-    <row r="376" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A376" s="1">
         <v>41183</v>
       </c>
@@ -4502,7 +4508,7 @@
         <v>1.0548999999999999</v>
       </c>
     </row>
-    <row r="377" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A377" s="1">
         <v>41183</v>
       </c>
@@ -4513,7 +4519,7 @@
         <v>1.1561999999999999</v>
       </c>
     </row>
-    <row r="378" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A378" s="1">
         <v>41183</v>
       </c>
@@ -4524,7 +4530,7 @@
         <v>4.1421999999999999</v>
       </c>
     </row>
-    <row r="379" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A379" s="1">
         <v>41183</v>
       </c>
@@ -4535,7 +4541,7 @@
         <v>3.0867</v>
       </c>
     </row>
-    <row r="380" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A380" s="1">
         <v>41183</v>
       </c>
@@ -4546,7 +4552,7 @@
         <v>7.2241</v>
       </c>
     </row>
-    <row r="381" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A381" s="1">
         <v>41183</v>
       </c>
@@ -4557,7 +4563,7 @@
         <v>5.3026</v>
       </c>
     </row>
-    <row r="382" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A382" s="1">
         <v>41183</v>
       </c>
@@ -4568,7 +4574,7 @@
         <v>5.3055000000000003</v>
       </c>
     </row>
-    <row r="383" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A383" s="1">
         <v>41183</v>
       </c>
@@ -4579,7 +4585,7 @@
         <v>8.2888999999999999</v>
       </c>
     </row>
-    <row r="384" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A384" s="1">
         <v>41183</v>
       </c>
@@ -4590,7 +4596,7 @@
         <v>3.0988000000000002</v>
       </c>
     </row>
-    <row r="385" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A385" s="1">
         <v>41183</v>
       </c>
@@ -4601,7 +4607,7 @@
         <v>4.1588000000000003</v>
       </c>
     </row>
-    <row r="386" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A386" s="1">
         <v>41183</v>
       </c>
@@ -4612,7 +4618,7 @@
         <v>1.0841000000000001</v>
       </c>
     </row>
-    <row r="387" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A387" s="1">
         <v>41183</v>
       </c>
@@ -4623,7 +4629,7 @@
         <v>4.2601000000000004</v>
       </c>
     </row>
-    <row r="388" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A388" s="1">
         <v>41183</v>
       </c>
@@ -4634,7 +4640,7 @@
         <v>5.3204000000000002</v>
       </c>
     </row>
-    <row r="389" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A389" s="1">
         <v>41183</v>
       </c>
@@ -4645,7 +4651,7 @@
         <v>3.1111</v>
       </c>
     </row>
-    <row r="390" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A390" s="1">
         <v>41183</v>
       </c>
@@ -4656,7 +4662,7 @@
         <v>2.0558999999999998</v>
       </c>
     </row>
-    <row r="391" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A391" s="1">
         <v>41183</v>
       </c>
@@ -4667,7 +4673,7 @@
         <v>5.2317</v>
       </c>
     </row>
-    <row r="392" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A392" s="1">
         <v>41183</v>
       </c>
@@ -4678,7 +4684,7 @@
         <v>1.0031000000000001</v>
       </c>
     </row>
-    <row r="393" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A393" s="1">
         <v>41183</v>
       </c>
@@ -4689,7 +4695,7 @@
         <v>1.2001999999999999</v>
       </c>
     </row>
-    <row r="394" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A394" s="1">
         <v>41183</v>
       </c>
@@ -4700,7 +4706,7 @@
         <v>1.2024999999999999</v>
       </c>
     </row>
-    <row r="395" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A395" s="1">
         <v>41183</v>
       </c>
@@ -4711,7 +4717,7 @@
         <v>1.2051000000000001</v>
       </c>
     </row>
-    <row r="396" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A396" s="1">
         <v>41183</v>
       </c>
@@ -4722,7 +4728,7 @@
         <v>1.2074</v>
       </c>
     </row>
-    <row r="397" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A397" s="1">
         <v>41183</v>
       </c>
@@ -4733,7 +4739,7 @@
         <v>2.2673999999999999</v>
       </c>
     </row>
-    <row r="398" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A398" s="1">
         <v>41183</v>
       </c>
@@ -4744,7 +4750,7 @@
         <v>2.1738</v>
       </c>
     </row>
-    <row r="399" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A399" s="1">
         <v>41183</v>
       </c>
@@ -4755,7 +4761,7 @@
         <v>4.2918000000000003</v>
       </c>
     </row>
-    <row r="400" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A400" s="1">
         <v>41183</v>
       </c>
@@ -4766,7 +4772,7 @@
         <v>3.1402999999999999</v>
       </c>
     </row>
-    <row r="401" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A401" s="1">
         <v>41183</v>
       </c>
@@ -4777,7 +4783,7 @@
         <v>2.0848</v>
       </c>
     </row>
-    <row r="402" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A402" s="1">
         <v>41183</v>
       </c>
@@ -4788,7 +4794,7 @@
         <v>1.1281000000000001</v>
       </c>
     </row>
-    <row r="403" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A403" s="1">
         <v>41183</v>
       </c>
@@ -4799,7 +4805,7 @@
         <v>2.1907000000000001</v>
       </c>
     </row>
-    <row r="404" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A404" s="1">
         <v>41183</v>
       </c>
@@ -4810,7 +4816,7 @@
         <v>1.2369000000000001</v>
       </c>
     </row>
-    <row r="405" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A405" s="1">
         <v>41183</v>
       </c>
@@ -4821,7 +4827,7 @@
         <v>1.1456</v>
       </c>
     </row>
-    <row r="406" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A406" s="1">
         <v>41183</v>
       </c>
@@ -4832,7 +4838,7 @@
         <v>1.1501999999999999</v>
       </c>
     </row>
-    <row r="407" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A407" s="1">
         <v>41214</v>
       </c>
@@ -4843,7 +4849,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="408" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A408" s="1">
         <v>41214</v>
       </c>
@@ -4854,7 +4860,7 @@
         <v>1.9630000000000001</v>
       </c>
     </row>
-    <row r="409" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A409" s="1">
         <v>41214</v>
       </c>
@@ -4865,7 +4871,7 @@
         <v>1.9630000000000001</v>
       </c>
     </row>
-    <row r="410" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A410" s="1">
         <v>41214</v>
       </c>
@@ -4876,7 +4882,7 @@
         <v>1.9630000000000001</v>
       </c>
     </row>
-    <row r="411" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A411" s="1">
         <v>41214</v>
       </c>
@@ -4887,7 +4893,7 @@
         <v>1.9630000000000001</v>
       </c>
     </row>
-    <row r="412" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A412" s="1">
         <v>41214</v>
       </c>
@@ -4898,7 +4904,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="413" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A413" s="1">
         <v>41214</v>
       </c>
@@ -4909,7 +4915,7 @@
         <v>1.9258999999999999</v>
       </c>
     </row>
-    <row r="414" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A414" s="1">
         <v>41214</v>
       </c>
@@ -4920,7 +4926,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="415" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A415" s="1">
         <v>41214</v>
       </c>
@@ -4931,7 +4937,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="416" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A416" s="1">
         <v>41214</v>
       </c>
@@ -4942,7 +4948,7 @@
         <v>3.0369999999999999</v>
       </c>
     </row>
-    <row r="417" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A417" s="1">
         <v>41214</v>
       </c>
@@ -4953,7 +4959,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="418" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A418" s="1">
         <v>41214</v>
       </c>
@@ -4964,7 +4970,7 @@
         <v>1.9630000000000001</v>
       </c>
     </row>
-    <row r="419" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A419" s="1">
         <v>41214</v>
       </c>
@@ -4975,7 +4981,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="420" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A420" s="1">
         <v>41214</v>
       </c>
@@ -4986,7 +4992,7 @@
         <v>1.0741000000000001</v>
       </c>
     </row>
-    <row r="421" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A421" s="1">
         <v>41214</v>
       </c>
@@ -4997,7 +5003,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="422" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A422" s="1">
         <v>41214</v>
       </c>
@@ -5008,7 +5014,7 @@
         <v>1.9630000000000001</v>
       </c>
     </row>
-    <row r="423" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A423" s="1">
         <v>41214</v>
       </c>
@@ -5019,7 +5025,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="424" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A424" s="1">
         <v>41214</v>
       </c>
@@ -5030,7 +5036,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="425" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A425" s="1">
         <v>41214</v>
       </c>
@@ -5041,7 +5047,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="426" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A426" s="1">
         <v>41214</v>
       </c>
@@ -5052,7 +5058,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="427" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A427" s="1">
         <v>41214</v>
       </c>
@@ -5063,7 +5069,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="428" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A428" s="1">
         <v>41214</v>
       </c>
@@ -5074,7 +5080,7 @@
         <v>0.96296000000000004</v>
       </c>
     </row>
-    <row r="429" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A429" s="1">
         <v>41214</v>
       </c>
@@ -5085,7 +5091,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="430" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A430" s="1">
         <v>41214</v>
       </c>
@@ -5096,7 +5102,7 @@
         <v>3.2593000000000001</v>
       </c>
     </row>
-    <row r="431" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A431" s="1">
         <v>41214</v>
       </c>
@@ -5107,7 +5113,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="432" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A432" s="1">
         <v>41214</v>
       </c>
@@ -5118,7 +5124,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="433" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A433" s="1">
         <v>41214</v>
       </c>
@@ -5129,7 +5135,7 @@
         <v>1.0369999999999999</v>
       </c>
     </row>
-    <row r="434" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A434" s="1">
         <v>41214</v>
       </c>
@@ -5140,7 +5146,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="435" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A435" s="1">
         <v>41214</v>
       </c>
@@ -5151,7 +5157,7 @@
         <v>1.0369999999999999</v>
       </c>
     </row>
-    <row r="436" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A436" s="1">
         <v>41214</v>
       </c>
@@ -5162,7 +5168,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="437" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A437" s="1">
         <v>41214</v>
       </c>
@@ -5173,7 +5179,7 @@
         <v>2.0369999999999999</v>
       </c>
     </row>
-    <row r="438" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A438" s="1">
         <v>41214</v>
       </c>
@@ -5184,7 +5190,7 @@
         <v>1.0369999999999999</v>
       </c>
     </row>
-    <row r="439" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A439" s="1">
         <v>41214</v>
       </c>
@@ -5195,7 +5201,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="440" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A440" s="1">
         <v>41214</v>
       </c>
@@ -5206,7 +5212,7 @@
         <v>1.9630000000000001</v>
       </c>
     </row>
-    <row r="441" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A441" s="1">
         <v>41214</v>
       </c>
@@ -5217,7 +5223,7 @@
         <v>1.9630000000000001</v>
       </c>
     </row>
-    <row r="442" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A442" s="1">
         <v>41214</v>
       </c>
@@ -5228,7 +5234,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="443" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A443" s="1">
         <v>41214</v>
       </c>
@@ -5239,7 +5245,7 @@
         <v>1.9258999999999999</v>
       </c>
     </row>
-    <row r="444" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A444" s="1">
         <v>41214</v>
       </c>
@@ -5250,7 +5256,7 @@
         <v>1.9630000000000001</v>
       </c>
     </row>
-    <row r="445" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A445" s="1">
         <v>41214</v>
       </c>
@@ -5261,7 +5267,7 @@
         <v>1.9630000000000001</v>
       </c>
     </row>
-    <row r="446" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A446" s="1">
         <v>41214</v>
       </c>
@@ -5272,7 +5278,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="447" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A447" s="1">
         <v>41214</v>
       </c>
@@ -5283,7 +5289,7 @@
         <v>1.0369999999999999</v>
       </c>
     </row>
-    <row r="448" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A448" s="1">
         <v>41214</v>
       </c>
@@ -5292,6 +5298,12 @@
       </c>
       <c r="C448" s="2">
         <v>1</v>
+      </c>
+    </row>
+    <row r="449" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C449">
+        <f>SUM(C2:C448)</f>
+        <v>2408.711470000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>